<commit_message>
[ADD] Changes added to export bills
</commit_message>
<xml_diff>
--- a/BillsInfo.xlsx
+++ b/BillsInfo.xlsx
@@ -524,12 +524,12 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>117.51</t>
+          <t>1175.10</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>117.51</t>
+          <t>1175.10</t>
         </is>
       </c>
     </row>
@@ -571,12 +571,12 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>75.03</t>
+          <t>1125.45</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>75.03</t>
+          <t>1125.45</t>
         </is>
       </c>
     </row>
@@ -588,7 +588,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>192.54</t>
+          <t>2300.55</t>
         </is>
       </c>
     </row>

</xml_diff>